<commit_message>
Se generan ficheros de produccion para 3ra produccion SETI
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CONNECTOR.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CONNECTOR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER-1K/02.BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER R-1/02.BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86021842-7470-234A-9076-3FA13901FE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F50B3D1-FB97-ED4C-95A9-0B887A8492AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Qty</t>
   </si>
@@ -88,9 +88,6 @@
     <t>NEW</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>Transistor</t>
   </si>
   <si>
@@ -173,6 +170,12 @@
   </si>
   <si>
     <t>VERSION</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Se actualiza columna NEW para nueva produccion SETI</t>
   </si>
 </sst>
 </file>
@@ -905,6 +908,10 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -917,10 +924,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1377,7 +1380,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1398,12 +1401,12 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="22">
+      <c r="B2" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="18">
         <f>MAX(_HISTORY!A4:A42)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="26" x14ac:dyDescent="0.25">
@@ -1413,12 +1416,12 @@
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="26" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
@@ -1457,7 +1460,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1466,16 +1469,16 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
         <v>40</v>
       </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" t="s">
-        <v>41</v>
-      </c>
       <c r="H7" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1483,7 +1486,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1495,7 +1498,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>13</v>
@@ -1506,7 +1509,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1518,10 +1521,10 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>14</v>
@@ -1555,10 +1558,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F394E835-0523-104C-AA22-72C38CD42C08}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1568,21 +1571,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="C3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="17" t="s">
         <v>24</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1593,10 +1596,10 @@
         <v>44874</v>
       </c>
       <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
         <v>37</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1607,10 +1610,10 @@
         <v>44880</v>
       </c>
       <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
         <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1618,13 +1621,27 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="10">
+        <v>45195</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1643,22 +1660,22 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="A1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="12"/>
@@ -1672,14 +1689,14 @@
     </row>
     <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -1691,19 +1708,19 @@
     </row>
     <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>36</v>
       </c>
       <c r="C9" s="12"/>
     </row>

</xml_diff>

<commit_message>
MOSFET de Salida cerrado permanentemente #87.
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CONNECTOR.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CONNECTOR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER R-1/02.BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DF5F23-939C-734F-8490-76A3FCFB1E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A128C3DF-9A0A-48B3-81A6-22286450CFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_CONNECTOR" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
   <si>
     <t>Qty</t>
   </si>
@@ -185,6 +185,24 @@
   </si>
   <si>
     <t>Se añade sustitutivo en pos 3</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>N.C</t>
+  </si>
+  <si>
+    <t>PTC</t>
+  </si>
+  <si>
+    <t>SMD 0805</t>
+  </si>
+  <si>
+    <t>Se añade part R1 en pos 4 con valor N.C</t>
   </si>
 </sst>
 </file>
@@ -876,7 +894,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -921,6 +939,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -933,54 +952,79 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1071,7 +1115,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:I10" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:I10" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="A6:I10" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:I10">
     <sortCondition ref="D6:D10"/>
@@ -1092,9 +1136,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1132,7 +1176,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1238,7 +1282,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1380,7 +1424,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1388,28 +1432,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
     <col min="9" max="9" width="146" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1418,30 +1462,30 @@
       </c>
       <c r="C2" s="18">
         <f>MAX(_HISTORY!A4:A42)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="26" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="27" x14ac:dyDescent="0.4">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="26" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+    <row r="4" spans="1:9" ht="27" x14ac:dyDescent="0.4">
+      <c r="B4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
-    </row>
-    <row r="5" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
@@ -1470,7 +1514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1496,7 +1540,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1519,7 +1563,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1546,21 +1590,44 @@
       </c>
       <c r="I9" s="9" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B4:E4"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:B9">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
+  <conditionalFormatting sqref="B6:B19">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="YES">
+      <formula>NOT(ISERROR(SEARCH("YES",B6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="YES">
-      <formula>NOT(ISERROR(SEARCH("YES",B7)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",B6)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -1577,23 +1644,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F394E835-0523-104C-AA22-72C38CD42C08}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>21</v>
       </c>
@@ -1607,7 +1674,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1621,7 +1688,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1635,7 +1702,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1649,7 +1716,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1663,11 +1730,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="20">
         <v>45245</v>
       </c>
       <c r="C8" t="s">
@@ -1675,6 +1742,20 @@
       </c>
       <c r="D8" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="25">
+        <v>45540</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1690,56 +1771,56 @@
       <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-    </row>
-    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="12"/>
     </row>
-    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>28805</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
     </row>
-    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>32</v>
       </c>
@@ -1748,7 +1829,7 @@
       </c>
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Connectores. Se añaden PADs para señales de comunicacion.
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CONNECTOR.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CONNECTOR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A128C3DF-9A0A-48B3-81A6-22286450CFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD459E78-8FE0-4AEC-B358-E0AD08AAF924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Qty</t>
   </si>
@@ -185,24 +185,6 @@
   </si>
   <si>
     <t>Se añade sustitutivo en pos 3</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>N.C</t>
-  </si>
-  <si>
-    <t>PTC</t>
-  </si>
-  <si>
-    <t>SMD 0805</t>
-  </si>
-  <si>
-    <t>Se añade part R1 en pos 4 con valor N.C</t>
   </si>
 </sst>
 </file>
@@ -894,7 +876,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -952,7 +934,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -999,32 +980,7 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1115,10 +1071,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:I10" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A6:I10" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:I10">
-    <sortCondition ref="D6:D10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:I9" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A6:I9" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:I9">
+    <sortCondition ref="D6:D9"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A4EEF5D5-EC32-4E92-A16D-A2C00D09EC58}" name="Position"/>
@@ -1432,10 +1388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,8 +1417,8 @@
         <v>44</v>
       </c>
       <c r="C2" s="18">
-        <f>MAX(_HISTORY!A4:A42)</f>
-        <v>6</v>
+        <f>MAX(_HISTORY!A4:A41)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="27" x14ac:dyDescent="0.4">
@@ -1592,39 +1548,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" t="s">
-        <v>54</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B4:E4"/>
   </mergeCells>
-  <conditionalFormatting sqref="B6:B19">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="YES">
+  <conditionalFormatting sqref="B6:B18">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",B6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",B6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",B6)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B6)))</formula>
@@ -1644,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F394E835-0523-104C-AA22-72C38CD42C08}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1742,20 +1675,6 @@
       </c>
       <c r="D8" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" s="25">
-        <v>45540</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>